<commit_message>
Add Reset form; Alert message & Stop button 5 seconds before importing
Update French & Spanish translations
Version 1.1
</commit_message>
<xml_diff>
--- a/tests/Students_RosarioSIS_test.xlsx
+++ b/tests/Students_RosarioSIS_test.xlsx
@@ -68,7 +68,7 @@
     <t xml:space="preserve">Female</t>
   </si>
   <si>
-    <t xml:space="preserve">merryl@strip.com</t>
+    <t xml:space="preserve">merryl@streep.com</t>
   </si>
   <si>
     <t xml:space="preserve">Roger</t>
@@ -140,7 +140,7 @@
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -179,12 +179,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +225,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -249,10 +243,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -284,18 +274,18 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8380566801619"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.82995951417"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2753036437247"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="22.3805668016194"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0364372469636"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -393,7 +383,7 @@
       <c r="A5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -401,7 +391,7 @@
       <c r="B6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -415,7 +405,7 @@
       <c r="C7" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="5" t="n">
         <v>37856</v>
       </c>
       <c r="F7" s="0" t="n">
@@ -435,7 +425,7 @@
       <c r="C8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>41042</v>
       </c>
       <c r="E8" s="0" t="n">
@@ -468,7 +458,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="john@smith.com"/>
-    <hyperlink ref="G3" r:id="rId2" display="merryl@strip.com"/>
+    <hyperlink ref="G3" r:id="rId2" display="merryl@streep.com"/>
     <hyperlink ref="G4" r:id="rId3" display="roger@rabbit.com"/>
     <hyperlink ref="G6" r:id="rId4" display="not@imported.com"/>
     <hyperlink ref="G7" r:id="rId5" display="no@accountnumber.com"/>

</xml_diff>